<commit_message>
Implemented dynamic selection between Class and Job lvl
</commit_message>
<xml_diff>
--- a/ragnarok/testes unitarios/excelstring.xlsx
+++ b/ragnarok/testes unitarios/excelstring.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Meus Documentos\Documentos\GitHub\ragna_calculator\ragnarok\testes unitarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA3BD99-FD2D-4F5D-A8FD-F0B1702E8E27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AEE026-7171-44DF-B62B-6C0FE4BACE63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="1065" windowWidth="25605" windowHeight="14325" activeTab="1" xr2:uid="{3DADE932-2264-4556-949F-E1022D134DF3}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="26">
   <si>
     <t>ATQ</t>
   </si>
@@ -94,10 +94,16 @@
     <t>&lt;/option&gt;</t>
   </si>
   <si>
-    <t>Novice</t>
+    <t>[</t>
   </si>
   <si>
-    <t>Super novice</t>
+    <t>["</t>
+  </si>
+  <si>
+    <t>", "</t>
+  </si>
+  <si>
+    <t>99"]</t>
   </si>
 </sst>
 </file>
@@ -2344,27 +2350,1211 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50F81730-FB13-4DDB-B2EB-2CB12D9FD72A}">
-  <dimension ref="B1:B3"/>
+  <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="F1" t="str">
+        <f>CONCATENATE(D1,D2,D3,D4,D5,D6,D7,D8,D9,D10,D11,D12,D13,D14,D15,D16,D17,D18,D19,D20,D21,D22,D23,D24,D25,D26,D27,D28,D29,D30,D31,D32,D33,D34,D35,D36,D37,D38,D39,D40,D41,D42,D43,D44,D45,D46,D47,D48,D49,D50,D51,D52,D53,D54,D55,D56,D57,D58,D59,D60,D61,D62,D63,D64,D65,D66,D67,D68,D69,D70,D71,D72,D73,D74,D75,D76,D77,D78,D79,D80,D81,D82,D83,D84,D85,D86,D87,D88,D89,D90,D91,D92,D93,D94,D95,D96,D97,D98,D99,D100)</f>
+        <v>[1", "2", "3", "4", "5", "6", "7", "8", "9", "10", "11", "12", "13", "14", "15", "16", "17", "18", "19", "20", "21", "22", "23", "24", "25", "26", "27", "28", "29", "30", "31", "32", "33", "34", "35", "36", "37", "38", "39", "40", "41", "42", "43", "44", "45", "46", "47", "48", "49", "50", "51", "52", "53", "54", "55", "56", "57", "58", "59", "60", "61", "62", "63", "64", "65", "66", "67", "68", "69", "70", "71", "72", "73", "74", "75", "76", "77", "78", "79", "80", "81", "82", "83", "84", "85", "86", "87", "88", "89", "90", "91", "92", "93", "94", "95", "96", "97", "98", "99"]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="str">
+        <f>CONCATENATE(A2, B2)</f>
+        <v>1", "</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="str">
+        <f>CONCATENATE(A3, B3)</f>
+        <v>2", "</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="str">
+        <f>CONCATENATE(A4, B4)</f>
+        <v>3", "</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="str">
+        <f>CONCATENATE(A5, B5)</f>
+        <v>4", "</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" ref="D6:D69" si="0">CONCATENATE(A6, B6)</f>
+        <v>5", "</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>6", "</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>7", "</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>8", "</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>9", "</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>10", "</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>11", "</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>12", "</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>13", "</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>14", "</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>15", "</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>16", "</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>17", "</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>18", "</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>19", "</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>20", "</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>21", "</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>22", "</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>23</v>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>23", "</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>24", "</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>25", "</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>26", "</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>27", "</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>28", "</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>29", "</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>30", "</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>31", "</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>32", "</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>33", "</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>34", "</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>35", "</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>36", "</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>37", "</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>38", "</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v>39", "</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v>40", "</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>24</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v>41", "</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v>42", "</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v>43", "</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>24</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v>44", "</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>24</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v>45", "</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>24</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="0"/>
+        <v>46", "</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>24</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="0"/>
+        <v>47", "</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>24</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="0"/>
+        <v>48", "</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>24</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="0"/>
+        <v>49", "</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>24</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="0"/>
+        <v>50", "</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>24</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="0"/>
+        <v>51", "</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>24</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="0"/>
+        <v>52", "</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>24</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="0"/>
+        <v>53", "</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>24</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="0"/>
+        <v>54", "</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>24</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="0"/>
+        <v>55", "</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>24</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="0"/>
+        <v>56", "</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>24</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="0"/>
+        <v>57", "</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>24</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="0"/>
+        <v>58", "</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>24</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="0"/>
+        <v>59", "</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>24</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="0"/>
+        <v>60", "</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>24</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="0"/>
+        <v>61", "</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>24</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="0"/>
+        <v>62", "</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>24</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="0"/>
+        <v>63", "</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>24</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="0"/>
+        <v>64", "</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>24</v>
+      </c>
+      <c r="D66" t="str">
+        <f t="shared" si="0"/>
+        <v>65", "</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>24</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" si="0"/>
+        <v>66", "</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>24</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="0"/>
+        <v>67", "</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>24</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" si="0"/>
+        <v>68", "</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>24</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" ref="D70:D100" si="1">CONCATENATE(A70, B70)</f>
+        <v>69", "</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>24</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="1"/>
+        <v>70", "</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>24</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" si="1"/>
+        <v>71", "</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>24</v>
+      </c>
+      <c r="D73" t="str">
+        <f t="shared" si="1"/>
+        <v>72", "</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>24</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="1"/>
+        <v>73", "</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>24</v>
+      </c>
+      <c r="D75" t="str">
+        <f t="shared" si="1"/>
+        <v>74", "</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>24</v>
+      </c>
+      <c r="D76" t="str">
+        <f t="shared" si="1"/>
+        <v>75", "</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>24</v>
+      </c>
+      <c r="D77" t="str">
+        <f t="shared" si="1"/>
+        <v>76", "</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>24</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" si="1"/>
+        <v>77", "</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>24</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" si="1"/>
+        <v>78", "</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>24</v>
+      </c>
+      <c r="D80" t="str">
+        <f t="shared" si="1"/>
+        <v>79", "</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>24</v>
+      </c>
+      <c r="D81" t="str">
+        <f t="shared" si="1"/>
+        <v>80", "</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>24</v>
+      </c>
+      <c r="D82" t="str">
+        <f t="shared" si="1"/>
+        <v>81", "</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>24</v>
+      </c>
+      <c r="D83" t="str">
+        <f t="shared" si="1"/>
+        <v>82", "</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>24</v>
+      </c>
+      <c r="D84" t="str">
+        <f t="shared" si="1"/>
+        <v>83", "</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>24</v>
+      </c>
+      <c r="D85" t="str">
+        <f t="shared" si="1"/>
+        <v>84", "</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>24</v>
+      </c>
+      <c r="D86" t="str">
+        <f t="shared" si="1"/>
+        <v>85", "</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>24</v>
+      </c>
+      <c r="D87" t="str">
+        <f t="shared" si="1"/>
+        <v>86", "</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>24</v>
+      </c>
+      <c r="D88" t="str">
+        <f t="shared" si="1"/>
+        <v>87", "</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>24</v>
+      </c>
+      <c r="D89" t="str">
+        <f t="shared" si="1"/>
+        <v>88", "</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>24</v>
+      </c>
+      <c r="D90" t="str">
+        <f t="shared" si="1"/>
+        <v>89", "</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>24</v>
+      </c>
+      <c r="D91" t="str">
+        <f t="shared" si="1"/>
+        <v>90", "</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>24</v>
+      </c>
+      <c r="D92" t="str">
+        <f t="shared" si="1"/>
+        <v>91", "</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>24</v>
+      </c>
+      <c r="D93" t="str">
+        <f t="shared" si="1"/>
+        <v>92", "</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>24</v>
+      </c>
+      <c r="D94" t="str">
+        <f t="shared" si="1"/>
+        <v>93", "</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>24</v>
+      </c>
+      <c r="D95" t="str">
+        <f t="shared" si="1"/>
+        <v>94", "</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>24</v>
+      </c>
+      <c r="D96" t="str">
+        <f t="shared" si="1"/>
+        <v>95", "</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>24</v>
+      </c>
+      <c r="D97" t="str">
+        <f t="shared" si="1"/>
+        <v>96", "</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>24</v>
+      </c>
+      <c r="D98" t="str">
+        <f t="shared" si="1"/>
+        <v>97", "</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>24</v>
+      </c>
+      <c r="D99" t="str">
+        <f t="shared" si="1"/>
+        <v>98", "</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>24</v>
+      </c>
+      <c r="D100" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>